<commit_message>
push pour déployement ajustement du fichier requirements.txt
</commit_message>
<xml_diff>
--- a/exports/releve.xlsx
+++ b/exports/releve.xlsx
@@ -14,29 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Banque</t>
   </si>
   <si>
-    <t>07" February 2014 International Bank Account Number</t>
+    <t>AFRILAND FIRST BANK</t>
   </si>
   <si>
     <t>Compte</t>
   </si>
   <si>
-    <t>00990275</t>
+    <t>0823752100109</t>
   </si>
   <si>
     <t>Titulaire</t>
   </si>
   <si>
-    <t>a</t>
+    <t>SAFIR CONSULTING CAMEROUN</t>
   </si>
   <si>
     <t>Période</t>
   </si>
   <si>
+    <t>02/03/2025 - 02/01/2025</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -49,43 +52,73 @@
     <t>Sens</t>
   </si>
   <si>
-    <t>14 Fob 13</t>
-  </si>
-  <si>
-    <t>Payment i NatWest Mage Debit ,000,000.00 3,700,000,000.00 Pay Ref 001887905 2B Feb 13° Payment to UK provident Debit 200,000,000.00 31500,000.000,00 Fund! by Oraft OS Mar 13 Direct Debit HSC UK Debit 1,000.000.00000 2:500,000,000.00</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Dr</t>
-  </si>
-  <si>
-    <t>21 Mar 13</t>
-  </si>
-  <si>
-    <t>Received from Microsoft UK Credit ,00000000 2.800.000.0000 ‘Account 504%0649 29Mar 13 Transfer from Sort Code 20- Credit 500,000,000.00 3,300,000,000.00 10-53 08 Mayt3 Payment to Exon Mobil Debit 100.000.000.00 3,200,000.000.00 Unlimited 15May 13 Received from British Creat 55,000.00000 3,255,000,00000 Petroleum 29May 13 Payment to Board of Internal Debit 5,000,000.00 3,250,000,000.00 O2 uy 13 Direct Debit HSBC China Debit 10.000,000.00 3.240,000,000.00</t>
-  </si>
-  <si>
-    <t>Cr</t>
-  </si>
-  <si>
-    <t>20 Aug 13</t>
-  </si>
-  <si>
-    <t>Received from Shell OP Cre .000.000.00 3,280,000.000.00 413.Sept 13° Drawn on Cho No. 448960 Debit 280,000.000.00 3,000,000,000.00 09.0ct 13. Transfer from HSBC Dubai Credit 100,000,000.00 3,100,000.000.00</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>07 Feb 14</t>
-  </si>
-  <si>
-    <t>Closing Balance ,100,000,000.00</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>02/01/2025</t>
+  </si>
+  <si>
+    <t>/24 PRELVALIOS FINANCE 12 1257225</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>/24 VIREMENT SALAIRE. 3 225 MENSUEL SAFI</t>
+  </si>
+  <si>
+    <t>03/09/2025</t>
+  </si>
+  <si>
+    <t>/24 FRAIS FIXE AU /24 5000 952.225</t>
+  </si>
+  <si>
+    <t>03/01/2025</t>
+  </si>
+  <si>
+    <t>/24 COMMISSION DE CPTE AU 107 BunzR4</t>
+  </si>
+  <si>
+    <t>/24 COMM. DE DECGUVERT AU 40 » 31224</t>
+  </si>
+  <si>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>0370172025 INTERETS DEBITEURS AU ( 909 771</t>
+  </si>
+  <si>
+    <t>28163</t>
+  </si>
+  <si>
+    <t>12/24</t>
+  </si>
+  <si>
+    <t>/24</t>
+  </si>
+  <si>
+    <t>3112</t>
+  </si>
+  <si>
+    <t>/24 TAXE/INTERETS OBT AU 54</t>
+  </si>
+  <si>
+    <t>03/01/2028</t>
+  </si>
+  <si>
+    <t>«/24 TX/COM. DECOUVERT Ais 7 31224</t>
+  </si>
+  <si>
+    <t>/24 TAXE COMM. DE CPTE AU 19 Bina</t>
+  </si>
+  <si>
+    <t>/24 TAXE FRAIS FIXE AU 9 B12</t>
+  </si>
+  <si>
+    <t>06/01/2025</t>
+  </si>
+  <si>
+    <t>/25 ViREMENT CIME BONA 11925, BBR 7IT</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
 </sst>
 </file>
@@ -417,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,72 +484,165 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>